<commit_message>
fixed bug in linear regression model, which did not compile (it used y instead of y_obs)
</commit_message>
<xml_diff>
--- a/syllabus/BDA-syllabus.xlsx
+++ b/syllabus/BDA-syllabus.xlsx
@@ -5,20 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A15378-2CA7-8B48-9497-529FFEB5BF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A8659C-427F-5F4F-89B8-07DEC29EA56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16000" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -96,9 +104,6 @@
     <t>esercizi da Ch 2 del libro</t>
   </si>
   <si>
-    <t>assignment 7 vekhtari (regressione pooled vs gerarchica)</t>
-  </si>
-  <si>
     <t>presentazione (o elaborazione) progetti</t>
   </si>
   <si>
@@ -108,9 +113,6 @@
     <t>exe da capitolo libro</t>
   </si>
   <si>
-    <t>buffer - flipped classRoom su AB test? (assegnare documentazione su eg 3 diversi aspetti di ab test) (to be seeen)</t>
-  </si>
-  <si>
     <t>test a due campioni per la proporzione (circa assignment 3. di vektari)</t>
   </si>
   <si>
@@ -151,13 +153,19 @@
   </si>
   <si>
     <t xml:space="preserve">ok come esercizio o anche assignment. Interessante: Frank Harrell’s recommendations on how to state results in Bayesian two group comparison. </t>
+  </si>
+  <si>
+    <t>attivtia' su AB test? (assegnare documentazione su eg 3 diversi aspetti di ab test) (to be seeen)</t>
+  </si>
+  <si>
+    <t>assignment 7 vekhtari (regressione logistica gerarchica su data set nuovo)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -181,13 +189,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <sz val="12"/>
@@ -196,8 +197,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,11 +224,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -224,20 +236,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -551,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D01C0E-36DF-B748-B91C-92F7CA25FEEF}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,17 +574,17 @@
     <col min="3" max="3" width="71.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -587,7 +598,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -598,7 +609,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -609,7 +620,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -620,7 +631,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -631,7 +642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -645,7 +656,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -656,7 +667,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -664,22 +675,26 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -687,24 +702,24 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -712,15 +727,15 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -728,10 +743,10 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -739,13 +754,13 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -753,10 +768,10 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -764,7 +779,7 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -772,10 +787,10 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -786,7 +801,7 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -794,7 +809,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -802,10 +817,10 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiornato syllabus dopo discussione con Marco
</commit_message>
<xml_diff>
--- a/syllabus/BDA-syllabus.xlsx
+++ b/syllabus/BDA-syllabus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A8659C-427F-5F4F-89B8-07DEC29EA56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A15495-C62F-344C-99A0-EE5634E624BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Settimana</t>
   </si>
@@ -47,12 +47,6 @@
     <t>linear regression</t>
   </si>
   <si>
-    <t>modelli lineari generalizzati</t>
-  </si>
-  <si>
-    <t>assignment 1: modello gerarchico factory; esercizio aggiuntivo; assignment 7-8 vehtari</t>
-  </si>
-  <si>
     <t>Bayesian t-test</t>
   </si>
   <si>
@@ -68,24 +62,12 @@
     <t>coin tossing, riportare la posterior</t>
   </si>
   <si>
-    <t>implementare metropolis, ad esempio per la normale</t>
-  </si>
-  <si>
     <t>assignment</t>
   </si>
   <si>
-    <t>distribuzioni, istogrammi, kde: vedi assignment 1 vekhtari</t>
-  </si>
-  <si>
-    <t>da assignment 1 vekhtari</t>
-  </si>
-  <si>
     <t>Bayes rule</t>
   </si>
   <si>
-    <t>sampling brute force riportando con che prob theta sta in un intervallo specifco</t>
-  </si>
-  <si>
     <t>metropolis (proporzione) e diagnostica</t>
   </si>
   <si>
@@ -95,39 +77,15 @@
     <t>Prob programming - multiparameter</t>
   </si>
   <si>
-    <t>lavoro su assignment?</t>
-  </si>
-  <si>
-    <t>bioassay con metropolis e comparare con pyMC3 - assigment 5 vekhtari</t>
-  </si>
-  <si>
-    <t>esercizi da Ch 2 del libro</t>
-  </si>
-  <si>
     <t>presentazione (o elaborazione) progetti</t>
   </si>
   <si>
     <t xml:space="preserve"> linear regression (robust-hier)</t>
   </si>
   <si>
-    <t>exe da capitolo libro</t>
-  </si>
-  <si>
-    <t>test a due campioni per la proporzione (circa assignment 3. di vektari)</t>
-  </si>
-  <si>
     <t>revisione progetti</t>
   </si>
   <si>
-    <t>esercizi collegati a bayesian t-test (campione a due test dipendenti?)</t>
-  </si>
-  <si>
-    <t>esercizio basato sulle 8 schols, fonnesbeck (regr lin gerarchica)</t>
-  </si>
-  <si>
-    <t>model selection (se ci sta..)</t>
-  </si>
-  <si>
     <t>Assignment vehtari</t>
   </si>
   <si>
@@ -155,10 +113,34 @@
     <t xml:space="preserve">ok come esercizio o anche assignment. Interessante: Frank Harrell’s recommendations on how to state results in Bayesian two group comparison. </t>
   </si>
   <si>
-    <t>attivtia' su AB test? (assegnare documentazione su eg 3 diversi aspetti di ab test) (to be seeen)</t>
-  </si>
-  <si>
-    <t>assignment 7 vekhtari (regressione logistica gerarchica su data set nuovo)</t>
+    <t>bioassay con metropolis; alcuni punti avanzati facoltativi; coprire nelle esercitazioni I pre-requisiti</t>
+  </si>
+  <si>
+    <t>distribuzioni, istogrammi, kde: bayes rule da assign 1 vekhtari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sampling brute force, uso del log, reporting della posterior (?) </t>
+  </si>
+  <si>
+    <t>metropolis (a mano vs pymc3)</t>
+  </si>
+  <si>
+    <t>attivtia' su AB test</t>
+  </si>
+  <si>
+    <t>linear regression (esercizi di martin)</t>
+  </si>
+  <si>
+    <t>regressione logistica</t>
+  </si>
+  <si>
+    <t>waic</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> modello gerarchico factory; esercizio aggiuntivo; assignment 7-8 vehtari</t>
   </si>
 </sst>
 </file>
@@ -214,7 +196,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,6 +206,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -240,13 +228,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -562,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D01C0E-36DF-B748-B91C-92F7CA25FEEF}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -574,17 +566,17 @@
     <col min="3" max="3" width="71.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -595,232 +587,232 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C9" s="8"/>
       <c r="D9" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>14</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="B25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" t="s">
-        <v>39</v>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
         <v>5</v>
       </c>
-      <c r="B27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>7</v>
-      </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>35</v>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
         <v>9</v>
       </c>
-      <c r="B31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" t="s">
-        <v>33</v>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated syllabus, including WAIC
</commit_message>
<xml_diff>
--- a/syllabus/BDA-syllabus.xlsx
+++ b/syllabus/BDA-syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A15495-C62F-344C-99A0-EE5634E624BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26D3F40-DBC3-1349-83F1-720B383DDC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
   </bookViews>
@@ -137,10 +137,10 @@
     <t>waic</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t xml:space="preserve"> modello gerarchico factory; esercizio aggiuntivo; assignment 7-8 vehtari</t>
+  </si>
+  <si>
+    <t>WAIC con calcolo via log sum exp,  statistical rethinking CH 7</t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -670,7 +670,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="6"/>
       <c r="F12" s="4"/>
@@ -722,7 +722,7 @@
         <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
bayes rule cleaned up, renamed as bayes rule, introduced goat
</commit_message>
<xml_diff>
--- a/syllabus/BDA-syllabus.xlsx
+++ b/syllabus/BDA-syllabus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26D3F40-DBC3-1349-83F1-720B383DDC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890EA8B0-B200-4146-93F9-F88955C6C2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
   </bookViews>

</xml_diff>

<commit_message>
updated reporting Bayesian analysis, now stable.
</commit_message>
<xml_diff>
--- a/syllabus/BDA-syllabus.xlsx
+++ b/syllabus/BDA-syllabus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890EA8B0-B200-4146-93F9-F88955C6C2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F507332-0F6A-4C43-83E5-5B47EB3F5359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
+    <workbookView xWindow="1600" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -128,9 +128,6 @@
     <t>attivtia' su AB test</t>
   </si>
   <si>
-    <t>linear regression (esercizi di martin)</t>
-  </si>
-  <si>
     <t>regressione logistica</t>
   </si>
   <si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>WAIC con calcolo via log sum exp,  statistical rethinking CH 7</t>
+  </si>
+  <si>
+    <t>linear regression (linear regression su un solo punto; esercizi di martin)</t>
   </si>
 </sst>
 </file>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D01C0E-36DF-B748-B91C-92F7CA25FEEF}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="184" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,7 +658,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="8"/>
     </row>
@@ -670,7 +670,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="6"/>
       <c r="F12" s="4"/>
@@ -695,7 +695,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D14" s="7"/>
     </row>
@@ -719,10 +719,10 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
minor update to  notebook 2- proporiton
</commit_message>
<xml_diff>
--- a/syllabus/BDA-syllabus.xlsx
+++ b/syllabus/BDA-syllabus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F507332-0F6A-4C43-83E5-5B47EB3F5359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332D8430-B8FD-7946-A948-69BF5663B273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>assignment</t>
   </si>
   <si>
-    <t>Bayes rule</t>
-  </si>
-  <si>
     <t>metropolis (proporzione) e diagnostica</t>
   </si>
   <si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>linear regression (linear regression su un solo punto; esercizi di martin)</t>
+  </si>
+  <si>
+    <t>Bayes rule (possibile caso di studio: The science of doping)</t>
   </si>
 </sst>
 </file>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D01C0E-36DF-B748-B91C-92F7CA25FEEF}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="184" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="184" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,10 +604,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -624,10 +624,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -635,11 +635,11 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -647,10 +647,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -658,7 +658,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="8"/>
     </row>
@@ -670,7 +670,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="6"/>
       <c r="F12" s="4"/>
@@ -682,7 +682,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="7"/>
@@ -695,7 +695,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="7"/>
     </row>
@@ -704,7 +704,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="6"/>
@@ -719,10 +719,10 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -735,10 +735,10 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -746,13 +746,13 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -760,10 +760,10 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
         <v>24</v>
-      </c>
-      <c r="C26" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -771,7 +771,7 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -779,10 +779,10 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" t="s">
         <v>22</v>
-      </c>
-      <c r="C28" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -793,7 +793,7 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -801,7 +801,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -809,10 +809,10 @@
         <v>9</v>
       </c>
       <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
         <v>18</v>
-      </c>
-      <c r="C32" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>